<commit_message>
End2End, but not yet with completed grid search..
</commit_message>
<xml_diff>
--- a/UvA/SensitivityAnalysis/Results.xlsx
+++ b/UvA/SensitivityAnalysis/Results.xlsx
@@ -479,22 +479,22 @@
         <v>64</v>
       </c>
       <c r="K2" t="n">
-        <v>0.6250315386700099</v>
+        <v>0.7887805686561092</v>
       </c>
       <c r="L2" t="n">
-        <v>0.8038437012194521</v>
+        <v>0.8680469733657697</v>
       </c>
       <c r="M2" t="n">
-        <v>0.831359143975096</v>
+        <v>0.886599188681837</v>
       </c>
       <c r="N2" t="n">
-        <v>0.6684440045047126</v>
+        <v>0.8136557880180363</v>
       </c>
       <c r="O2" t="n">
-        <v>0</v>
+        <v>2.421804666519165</v>
       </c>
       <c r="P2" t="n">
-        <v>0</v>
+        <v>9.87317681312561</v>
       </c>
     </row>
     <row r="3">
@@ -533,22 +533,22 @@
         <v>64</v>
       </c>
       <c r="K3" t="n">
-        <v>0.697170189666396</v>
+        <v>0.6406127450008707</v>
       </c>
       <c r="L3" t="n">
-        <v>0.8424787440701222</v>
+        <v>0.8085239579549567</v>
       </c>
       <c r="M3" t="n">
-        <v>0.8645591373128726</v>
+        <v>0.8353275031091926</v>
       </c>
       <c r="N3" t="n">
-        <v>0.732437433061254</v>
+        <v>0.6820897889154897</v>
       </c>
       <c r="O3" t="n">
-        <v>0</v>
+        <v>0.009971857070922852</v>
       </c>
       <c r="P3" t="n">
-        <v>0</v>
+        <v>17.88996005058289</v>
       </c>
     </row>
     <row r="4">
@@ -587,22 +587,22 @@
         <v>64</v>
       </c>
       <c r="K4" t="n">
-        <v>0.7289521766096944</v>
+        <v>0.6416683145038612</v>
       </c>
       <c r="L4" t="n">
-        <v>0.8363155308579242</v>
+        <v>0.8002198692333028</v>
       </c>
       <c r="M4" t="n">
-        <v>0.8593033004475922</v>
+        <v>0.8282415036296485</v>
       </c>
       <c r="N4" t="n">
-        <v>0.7606030754278906</v>
+        <v>0.6831840136352011</v>
       </c>
       <c r="O4" t="n">
-        <v>0</v>
+        <v>5.420705080032349</v>
       </c>
       <c r="P4" t="n">
-        <v>0</v>
+        <v>13.32115316390991</v>
       </c>
     </row>
     <row r="5">
@@ -641,22 +641,22 @@
         <v>64</v>
       </c>
       <c r="K5" t="n">
-        <v>0.7477503292134453</v>
+        <v>0.6474648589640518</v>
       </c>
       <c r="L5" t="n">
-        <v>0.8630415643779646</v>
+        <v>0.8116937274579437</v>
       </c>
       <c r="M5" t="n">
-        <v>0.8821799967741003</v>
+        <v>0.8381024182563098</v>
       </c>
       <c r="N5" t="n">
-        <v>0.7773391775322159</v>
+        <v>0.6884617519931663</v>
       </c>
       <c r="O5" t="n">
-        <v>0</v>
+        <v>0.01810789108276367</v>
       </c>
       <c r="P5" t="n">
-        <v>0</v>
+        <v>10.53526401519775</v>
       </c>
     </row>
     <row r="6">
@@ -695,22 +695,22 @@
         <v>64</v>
       </c>
       <c r="K6" t="n">
-        <v>0.6250315386700099</v>
+        <v>0.7543611620564029</v>
       </c>
       <c r="L6" t="n">
-        <v>0.8038437012194521</v>
+        <v>0.8247614623016217</v>
       </c>
       <c r="M6" t="n">
-        <v>0.831359143975096</v>
+        <v>0.8492930056684334</v>
       </c>
       <c r="N6" t="n">
-        <v>0.6684440045047126</v>
+        <v>0.7832130971824748</v>
       </c>
       <c r="O6" t="n">
-        <v>0</v>
+        <v>2.326012134552002</v>
       </c>
       <c r="P6" t="n">
-        <v>0</v>
+        <v>10.00130295753479</v>
       </c>
     </row>
     <row r="7">
@@ -749,22 +749,22 @@
         <v>64</v>
       </c>
       <c r="K7" t="n">
-        <v>0.697170189666396</v>
+        <v>0.7866866638067317</v>
       </c>
       <c r="L7" t="n">
-        <v>0.8424787440701222</v>
+        <v>0.8595642958532245</v>
       </c>
       <c r="M7" t="n">
-        <v>0.8645591373128726</v>
+        <v>0.8792428206668126</v>
       </c>
       <c r="N7" t="n">
-        <v>0.732437433061254</v>
+        <v>0.8117675522933305</v>
       </c>
       <c r="O7" t="n">
-        <v>0</v>
+        <v>0.01061010360717773</v>
       </c>
       <c r="P7" t="n">
-        <v>0</v>
+        <v>9.8405921459198</v>
       </c>
     </row>
     <row r="8">
@@ -803,22 +803,22 @@
         <v>64</v>
       </c>
       <c r="K8" t="n">
-        <v>0.7289521766096944</v>
+        <v>0.7618932795693877</v>
       </c>
       <c r="L8" t="n">
-        <v>0.8363155308579242</v>
+        <v>0.8381243637668739</v>
       </c>
       <c r="M8" t="n">
-        <v>0.8593033004475922</v>
+        <v>0.8607266686378819</v>
       </c>
       <c r="N8" t="n">
-        <v>0.7606030754278906</v>
+        <v>0.789868640210356</v>
       </c>
       <c r="O8" t="n">
-        <v>0</v>
+        <v>2.510090112686157</v>
       </c>
       <c r="P8" t="n">
-        <v>0</v>
+        <v>9.885471820831299</v>
       </c>
     </row>
     <row r="9">
@@ -857,22 +857,22 @@
         <v>64</v>
       </c>
       <c r="K9" t="n">
-        <v>0.7477503292134453</v>
+        <v>0.6501465437034426</v>
       </c>
       <c r="L9" t="n">
-        <v>0.8630415643779646</v>
+        <v>0.8169721950153157</v>
       </c>
       <c r="M9" t="n">
-        <v>0.8821799967741003</v>
+        <v>0.8425622134110246</v>
       </c>
       <c r="N9" t="n">
-        <v>0.7773391775322159</v>
+        <v>0.6904993654734219</v>
       </c>
       <c r="O9" t="n">
-        <v>0</v>
+        <v>0.01228117942810059</v>
       </c>
       <c r="P9" t="n">
-        <v>0</v>
+        <v>19.89185190200806</v>
       </c>
     </row>
   </sheetData>

</xml_diff>